<commit_message>
added specimen to bundle, required specimen for HLA profiles
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-MSBundle.xlsx
+++ b/docs/StructureDefinition-MSBundle.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AM$545</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AM$577</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18930" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20038" uniqueCount="453">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-06-29T21:07:13-05:00</t>
+    <t>2022-06-30T09:28:59-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1337,7 +1337,29 @@
     <t>This profile defines  how to represent body weight observations in FHIR using a standard LOINC code and UCUM units of measure.</t>
   </si>
   <si>
-    <t>hlaa</t>
+    <t>msSpecimen</t>
+  </si>
+  <si>
+    <t>Specimen used for HLA genotyping</t>
+  </si>
+  <si>
+    <t>Specimen used for HLA genotyping. The identifier found here can be used to link to an HML file if submitted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specimen {http://fhir.nmdp.org/ig/matchsource/StructureDefinition/msspecimen}
+</t>
+  </si>
+  <si>
+    <t>Sample for analysis</t>
+  </si>
+  <si>
+    <t>A sample to be used for analysis.</t>
+  </si>
+  <si>
+    <t>Role[classCode=SPEC]</t>
+  </si>
+  <si>
+    <t>hla-a</t>
   </si>
   <si>
     <t>HLA-A</t>
@@ -1353,7 +1375,7 @@
     <t>Genotype</t>
   </si>
   <si>
-    <t>hlab</t>
+    <t>hla-b</t>
   </si>
   <si>
     <t>HLA-B</t>
@@ -1366,7 +1388,7 @@
 </t>
   </si>
   <si>
-    <t>hlac</t>
+    <t>hla-c</t>
   </si>
   <si>
     <t>HLA-C</t>
@@ -1379,7 +1401,7 @@
 </t>
   </si>
   <si>
-    <t>hladrb1</t>
+    <t>hla-drb1</t>
   </si>
   <si>
     <t>HLA-DRB1</t>
@@ -1392,7 +1414,7 @@
 </t>
   </si>
   <si>
-    <t>hladpb1</t>
+    <t>hla-dpb1</t>
   </si>
   <si>
     <t>HLA-DPB1</t>
@@ -1733,7 +1755,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AM545"/>
+  <dimension ref="A1:AM577"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -44825,7 +44847,7 @@
       </c>
       <c r="B391" s="2"/>
       <c r="C391" t="s" s="2">
-        <v>387</v>
+        <v>74</v>
       </c>
       <c r="D391" s="2"/>
       <c r="E391" t="s" s="2">
@@ -44850,11 +44872,9 @@
         <v>423</v>
       </c>
       <c r="L391" t="s" s="2">
-        <v>390</v>
-      </c>
-      <c r="M391" t="s" s="2">
-        <v>391</v>
-      </c>
+        <v>424</v>
+      </c>
+      <c r="M391" s="2"/>
       <c r="N391" s="2"/>
       <c r="O391" t="s" s="2">
         <v>74</v>
@@ -44915,13 +44935,13 @@
         <v>74</v>
       </c>
       <c r="AI391" t="s" s="2">
-        <v>392</v>
+        <v>373</v>
       </c>
       <c r="AJ391" t="s" s="2">
-        <v>393</v>
+        <v>74</v>
       </c>
       <c r="AK391" t="s" s="2">
-        <v>394</v>
+        <v>425</v>
       </c>
       <c r="AL391" t="s" s="2">
         <v>74</v>
@@ -47690,7 +47710,7 @@
         <v>257</v>
       </c>
       <c r="B417" t="s" s="2">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="C417" t="s" s="2">
         <v>74</v>
@@ -47715,10 +47735,10 @@
         <v>239</v>
       </c>
       <c r="K417" t="s" s="2">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="L417" t="s" s="2">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="M417" s="2"/>
       <c r="N417" s="2"/>
@@ -48374,10 +48394,10 @@
         <v>74</v>
       </c>
       <c r="J423" t="s" s="2">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="K423" t="s" s="2">
-        <v>423</v>
+        <v>430</v>
       </c>
       <c r="L423" t="s" s="2">
         <v>390</v>
@@ -51220,7 +51240,7 @@
         <v>257</v>
       </c>
       <c r="B449" t="s" s="2">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="C449" t="s" s="2">
         <v>74</v>
@@ -51245,10 +51265,10 @@
         <v>239</v>
       </c>
       <c r="K449" t="s" s="2">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="L449" t="s" s="2">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="M449" s="2"/>
       <c r="N449" s="2"/>
@@ -51904,10 +51924,10 @@
         <v>74</v>
       </c>
       <c r="J455" t="s" s="2">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="K455" t="s" s="2">
-        <v>423</v>
+        <v>430</v>
       </c>
       <c r="L455" t="s" s="2">
         <v>390</v>
@@ -54750,7 +54770,7 @@
         <v>257</v>
       </c>
       <c r="B481" t="s" s="2">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="C481" t="s" s="2">
         <v>74</v>
@@ -54775,10 +54795,10 @@
         <v>239</v>
       </c>
       <c r="K481" t="s" s="2">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="L481" t="s" s="2">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="M481" s="2"/>
       <c r="N481" s="2"/>
@@ -55434,10 +55454,10 @@
         <v>74</v>
       </c>
       <c r="J487" t="s" s="2">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="K487" t="s" s="2">
-        <v>423</v>
+        <v>430</v>
       </c>
       <c r="L487" t="s" s="2">
         <v>390</v>
@@ -58280,7 +58300,7 @@
         <v>257</v>
       </c>
       <c r="B513" t="s" s="2">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="C513" t="s" s="2">
         <v>74</v>
@@ -58305,10 +58325,10 @@
         <v>239</v>
       </c>
       <c r="K513" t="s" s="2">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="L513" t="s" s="2">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="M513" s="2"/>
       <c r="N513" s="2"/>
@@ -58964,10 +58984,10 @@
         <v>74</v>
       </c>
       <c r="J519" t="s" s="2">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="K519" t="s" s="2">
-        <v>423</v>
+        <v>430</v>
       </c>
       <c r="L519" t="s" s="2">
         <v>390</v>
@@ -61805,11 +61825,13 @@
         <v>74</v>
       </c>
     </row>
-    <row r="545" hidden="true">
+    <row r="545">
       <c r="A545" t="s" s="2">
-        <v>440</v>
-      </c>
-      <c r="B545" s="2"/>
+        <v>257</v>
+      </c>
+      <c r="B545" t="s" s="2">
+        <v>443</v>
+      </c>
       <c r="C545" t="s" s="2">
         <v>74</v>
       </c>
@@ -61821,7 +61843,7 @@
         <v>83</v>
       </c>
       <c r="G545" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="H545" t="s" s="2">
         <v>74</v>
@@ -61830,20 +61852,16 @@
         <v>84</v>
       </c>
       <c r="J545" t="s" s="2">
-        <v>441</v>
+        <v>239</v>
       </c>
       <c r="K545" t="s" s="2">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="L545" t="s" s="2">
-        <v>443</v>
-      </c>
-      <c r="M545" t="s" s="2">
-        <v>444</v>
-      </c>
-      <c r="N545" t="s" s="2">
         <v>445</v>
       </c>
+      <c r="M545" s="2"/>
+      <c r="N545" s="2"/>
       <c r="O545" t="s" s="2">
         <v>74</v>
       </c>
@@ -61891,35 +61909,3567 @@
         <v>74</v>
       </c>
       <c r="AE545" t="s" s="2">
-        <v>440</v>
+        <v>257</v>
       </c>
       <c r="AF545" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG545" t="s" s="2">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="AH545" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AI545" t="s" s="2">
+        <v>263</v>
+      </c>
+      <c r="AJ545" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK545" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL545" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM545" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="546" hidden="true">
+      <c r="A546" t="s" s="2">
+        <v>264</v>
+      </c>
+      <c r="B546" s="2"/>
+      <c r="C546" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="D546" s="2"/>
+      <c r="E546" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F546" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="G546" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H546" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I546" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J546" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K546" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="L546" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="M546" s="2"/>
+      <c r="N546" s="2"/>
+      <c r="O546" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P546" s="2"/>
+      <c r="Q546" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R546" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S546" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T546" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U546" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V546" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W546" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X546" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y546" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z546" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA546" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB546" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC546" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD546" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE546" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AF546" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG546" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AH546" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI546" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AJ546" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK546" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="AL546" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM546" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="547" hidden="true">
+      <c r="A547" t="s" s="2">
+        <v>265</v>
+      </c>
+      <c r="B547" s="2"/>
+      <c r="C547" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="D547" s="2"/>
+      <c r="E547" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F547" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G547" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H547" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I547" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J547" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="K547" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="L547" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="M547" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="N547" s="2"/>
+      <c r="O547" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P547" s="2"/>
+      <c r="Q547" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R547" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S547" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T547" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U547" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V547" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W547" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X547" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y547" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z547" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA547" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB547" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC547" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD547" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE547" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="AF547" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG547" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH547" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI547" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="AJ547" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK547" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="AL547" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM547" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="548" hidden="true">
+      <c r="A548" t="s" s="2">
+        <v>266</v>
+      </c>
+      <c r="B548" s="2"/>
+      <c r="C548" t="s" s="2">
+        <v>246</v>
+      </c>
+      <c r="D548" s="2"/>
+      <c r="E548" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F548" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G548" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H548" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="I548" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="J548" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="K548" t="s" s="2">
+        <v>247</v>
+      </c>
+      <c r="L548" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="M548" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="N548" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="O548" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P548" s="2"/>
+      <c r="Q548" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R548" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S548" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T548" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U548" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V548" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W548" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X548" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y548" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z548" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA548" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB548" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC548" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD548" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE548" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="AF548" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG548" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH548" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI548" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="AJ548" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK548" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL548" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM548" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="549" hidden="true">
+      <c r="A549" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="B549" s="2"/>
+      <c r="C549" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="D549" s="2"/>
+      <c r="E549" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F549" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G549" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H549" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I549" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="J549" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="K549" t="s" s="2">
+        <v>268</v>
+      </c>
+      <c r="L549" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="M549" s="2"/>
+      <c r="N549" s="2"/>
+      <c r="O549" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P549" s="2"/>
+      <c r="Q549" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R549" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S549" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T549" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U549" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V549" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W549" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X549" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y549" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z549" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA549" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB549" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC549" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD549" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE549" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="AF549" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG549" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH549" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI549" t="s" s="2">
         <v>95</v>
       </c>
-      <c r="AJ545" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AK545" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AL545" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AM545" t="s" s="2">
+      <c r="AJ549" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK549" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL549" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM549" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="550" hidden="true">
+      <c r="A550" t="s" s="2">
+        <v>270</v>
+      </c>
+      <c r="B550" s="2"/>
+      <c r="C550" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="D550" s="2"/>
+      <c r="E550" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F550" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="G550" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H550" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I550" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="J550" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="K550" t="s" s="2">
+        <v>271</v>
+      </c>
+      <c r="L550" t="s" s="2">
+        <v>272</v>
+      </c>
+      <c r="M550" t="s" s="2">
+        <v>273</v>
+      </c>
+      <c r="N550" s="2"/>
+      <c r="O550" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P550" s="2"/>
+      <c r="Q550" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R550" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S550" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T550" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U550" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V550" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W550" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X550" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y550" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z550" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA550" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB550" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC550" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD550" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE550" t="s" s="2">
+        <v>270</v>
+      </c>
+      <c r="AF550" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG550" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AH550" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI550" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="AJ550" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK550" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL550" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM550" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="551" hidden="true">
+      <c r="A551" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="B551" s="2"/>
+      <c r="C551" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="D551" s="2"/>
+      <c r="E551" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F551" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="G551" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H551" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I551" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J551" t="s" s="2">
+        <v>446</v>
+      </c>
+      <c r="K551" t="s" s="2">
+        <v>430</v>
+      </c>
+      <c r="L551" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="M551" t="s" s="2">
+        <v>391</v>
+      </c>
+      <c r="N551" s="2"/>
+      <c r="O551" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P551" s="2"/>
+      <c r="Q551" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R551" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S551" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T551" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U551" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V551" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W551" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X551" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y551" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z551" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA551" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB551" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC551" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD551" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE551" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="AF551" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG551" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AH551" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI551" t="s" s="2">
+        <v>392</v>
+      </c>
+      <c r="AJ551" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="AK551" t="s" s="2">
+        <v>394</v>
+      </c>
+      <c r="AL551" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM551" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="552" hidden="true">
+      <c r="A552" t="s" s="2">
+        <v>278</v>
+      </c>
+      <c r="B552" s="2"/>
+      <c r="C552" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="D552" s="2"/>
+      <c r="E552" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F552" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="G552" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H552" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I552" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="J552" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="K552" t="s" s="2">
+        <v>279</v>
+      </c>
+      <c r="L552" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="M552" s="2"/>
+      <c r="N552" s="2"/>
+      <c r="O552" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P552" s="2"/>
+      <c r="Q552" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R552" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S552" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T552" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U552" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V552" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W552" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X552" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y552" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z552" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA552" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB552" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC552" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD552" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE552" t="s" s="2">
+        <v>278</v>
+      </c>
+      <c r="AF552" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG552" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AH552" t="s" s="2">
+        <v>281</v>
+      </c>
+      <c r="AI552" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="AJ552" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK552" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL552" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM552" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="553" hidden="true">
+      <c r="A553" t="s" s="2">
+        <v>282</v>
+      </c>
+      <c r="B553" s="2"/>
+      <c r="C553" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="D553" s="2"/>
+      <c r="E553" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F553" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="G553" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H553" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I553" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J553" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K553" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="L553" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="M553" s="2"/>
+      <c r="N553" s="2"/>
+      <c r="O553" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P553" s="2"/>
+      <c r="Q553" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R553" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S553" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T553" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U553" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V553" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W553" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X553" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y553" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z553" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA553" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB553" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC553" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD553" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE553" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AF553" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG553" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AH553" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI553" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AJ553" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK553" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="AL553" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM553" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="554" hidden="true">
+      <c r="A554" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="B554" s="2"/>
+      <c r="C554" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="D554" s="2"/>
+      <c r="E554" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F554" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G554" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H554" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I554" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J554" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="K554" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="L554" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="M554" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="N554" s="2"/>
+      <c r="O554" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P554" s="2"/>
+      <c r="Q554" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R554" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S554" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T554" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U554" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V554" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W554" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X554" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y554" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z554" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA554" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB554" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC554" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD554" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE554" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="AF554" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG554" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH554" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI554" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="AJ554" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK554" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="AL554" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM554" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="555" hidden="true">
+      <c r="A555" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="B555" s="2"/>
+      <c r="C555" t="s" s="2">
+        <v>246</v>
+      </c>
+      <c r="D555" s="2"/>
+      <c r="E555" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F555" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G555" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H555" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="I555" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="J555" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="K555" t="s" s="2">
+        <v>247</v>
+      </c>
+      <c r="L555" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="M555" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="N555" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="O555" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P555" s="2"/>
+      <c r="Q555" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R555" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S555" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T555" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U555" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V555" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W555" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X555" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y555" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z555" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA555" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB555" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC555" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD555" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE555" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="AF555" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG555" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH555" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI555" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="AJ555" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK555" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL555" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM555" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="556" hidden="true">
+      <c r="A556" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="B556" s="2"/>
+      <c r="C556" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="D556" s="2"/>
+      <c r="E556" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F556" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="G556" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H556" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I556" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="J556" t="s" s="2">
+        <v>167</v>
+      </c>
+      <c r="K556" t="s" s="2">
+        <v>286</v>
+      </c>
+      <c r="L556" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="M556" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="N556" s="2"/>
+      <c r="O556" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P556" s="2"/>
+      <c r="Q556" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R556" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S556" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T556" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U556" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V556" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W556" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="X556" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="Y556" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="Z556" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA556" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB556" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC556" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD556" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE556" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="AF556" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG556" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AH556" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI556" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="AJ556" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK556" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL556" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM556" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="557" hidden="true">
+      <c r="A557" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="B557" s="2"/>
+      <c r="C557" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="D557" s="2"/>
+      <c r="E557" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F557" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="G557" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H557" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I557" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="J557" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="K557" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="L557" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="M557" t="s" s="2">
+        <v>295</v>
+      </c>
+      <c r="N557" s="2"/>
+      <c r="O557" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P557" s="2"/>
+      <c r="Q557" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R557" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S557" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T557" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U557" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V557" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W557" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X557" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y557" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z557" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA557" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB557" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC557" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD557" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE557" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="AF557" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG557" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AH557" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI557" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="AJ557" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK557" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL557" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM557" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="558" hidden="true">
+      <c r="A558" t="s" s="2">
+        <v>296</v>
+      </c>
+      <c r="B558" s="2"/>
+      <c r="C558" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="D558" s="2"/>
+      <c r="E558" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F558" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="G558" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H558" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I558" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="J558" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="K558" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="L558" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="M558" s="2"/>
+      <c r="N558" s="2"/>
+      <c r="O558" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P558" s="2"/>
+      <c r="Q558" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R558" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S558" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T558" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U558" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V558" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W558" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X558" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y558" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z558" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA558" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB558" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC558" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD558" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE558" t="s" s="2">
+        <v>296</v>
+      </c>
+      <c r="AF558" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG558" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AH558" t="s" s="2">
+        <v>299</v>
+      </c>
+      <c r="AI558" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="AJ558" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK558" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL558" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM558" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="559" hidden="true">
+      <c r="A559" t="s" s="2">
+        <v>300</v>
+      </c>
+      <c r="B559" s="2"/>
+      <c r="C559" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="D559" s="2"/>
+      <c r="E559" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F559" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="G559" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H559" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I559" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J559" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K559" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="L559" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="M559" s="2"/>
+      <c r="N559" s="2"/>
+      <c r="O559" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P559" s="2"/>
+      <c r="Q559" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R559" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S559" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T559" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U559" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V559" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W559" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X559" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y559" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z559" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA559" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB559" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC559" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD559" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE559" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AF559" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG559" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AH559" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI559" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AJ559" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK559" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="AL559" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM559" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="560" hidden="true">
+      <c r="A560" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="B560" s="2"/>
+      <c r="C560" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="D560" s="2"/>
+      <c r="E560" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F560" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G560" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H560" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I560" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J560" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="K560" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="L560" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="M560" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="N560" s="2"/>
+      <c r="O560" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P560" s="2"/>
+      <c r="Q560" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R560" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S560" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T560" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U560" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V560" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W560" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X560" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y560" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z560" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA560" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB560" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC560" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD560" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE560" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="AF560" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG560" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH560" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI560" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="AJ560" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK560" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="AL560" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM560" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="561" hidden="true">
+      <c r="A561" t="s" s="2">
+        <v>302</v>
+      </c>
+      <c r="B561" s="2"/>
+      <c r="C561" t="s" s="2">
+        <v>246</v>
+      </c>
+      <c r="D561" s="2"/>
+      <c r="E561" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F561" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G561" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H561" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="I561" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="J561" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="K561" t="s" s="2">
+        <v>247</v>
+      </c>
+      <c r="L561" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="M561" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="N561" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="O561" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P561" s="2"/>
+      <c r="Q561" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R561" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S561" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T561" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U561" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V561" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W561" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X561" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y561" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z561" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA561" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB561" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC561" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD561" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE561" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="AF561" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG561" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH561" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI561" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="AJ561" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK561" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL561" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM561" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="562" hidden="true">
+      <c r="A562" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B562" s="2"/>
+      <c r="C562" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="D562" s="2"/>
+      <c r="E562" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="F562" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="G562" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H562" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I562" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="J562" t="s" s="2">
+        <v>167</v>
+      </c>
+      <c r="K562" t="s" s="2">
+        <v>304</v>
+      </c>
+      <c r="L562" t="s" s="2">
+        <v>305</v>
+      </c>
+      <c r="M562" s="2"/>
+      <c r="N562" s="2"/>
+      <c r="O562" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P562" s="2"/>
+      <c r="Q562" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R562" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S562" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T562" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U562" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V562" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W562" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="X562" t="s" s="2">
+        <v>306</v>
+      </c>
+      <c r="Y562" t="s" s="2">
+        <v>307</v>
+      </c>
+      <c r="Z562" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA562" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB562" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC562" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD562" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE562" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="AF562" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AG562" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AH562" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI562" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="AJ562" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK562" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL562" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM562" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="563" hidden="true">
+      <c r="A563" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="B563" s="2"/>
+      <c r="C563" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="D563" s="2"/>
+      <c r="E563" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="F563" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="G563" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H563" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I563" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="J563" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="K563" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="L563" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="M563" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="N563" s="2"/>
+      <c r="O563" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P563" s="2"/>
+      <c r="Q563" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R563" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S563" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T563" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U563" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V563" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W563" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X563" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y563" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z563" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA563" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB563" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC563" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD563" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE563" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="AF563" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AG563" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AH563" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI563" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="AJ563" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK563" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL563" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM563" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="564" hidden="true">
+      <c r="A564" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="B564" s="2"/>
+      <c r="C564" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="D564" s="2"/>
+      <c r="E564" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F564" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="G564" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H564" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I564" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="J564" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K564" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="L564" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="M564" s="2"/>
+      <c r="N564" s="2"/>
+      <c r="O564" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P564" s="2"/>
+      <c r="Q564" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R564" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S564" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T564" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U564" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V564" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W564" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X564" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y564" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z564" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA564" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB564" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC564" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD564" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE564" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="AF564" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG564" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AH564" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI564" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="AJ564" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK564" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL564" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM564" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="565" hidden="true">
+      <c r="A565" t="s" s="2">
+        <v>315</v>
+      </c>
+      <c r="B565" s="2"/>
+      <c r="C565" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="D565" s="2"/>
+      <c r="E565" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F565" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="G565" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H565" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I565" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="J565" t="s" s="2">
+        <v>119</v>
+      </c>
+      <c r="K565" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="L565" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="M565" s="2"/>
+      <c r="N565" s="2"/>
+      <c r="O565" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P565" s="2"/>
+      <c r="Q565" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R565" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S565" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T565" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U565" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V565" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W565" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X565" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y565" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z565" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA565" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB565" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC565" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD565" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE565" t="s" s="2">
+        <v>315</v>
+      </c>
+      <c r="AF565" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG565" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AH565" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI565" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="AJ565" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK565" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL565" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM565" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="566" hidden="true">
+      <c r="A566" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="B566" s="2"/>
+      <c r="C566" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="D566" s="2"/>
+      <c r="E566" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F566" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="G566" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H566" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I566" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="J566" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K566" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="L566" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="M566" s="2"/>
+      <c r="N566" s="2"/>
+      <c r="O566" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P566" s="2"/>
+      <c r="Q566" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R566" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S566" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T566" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U566" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V566" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W566" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X566" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y566" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z566" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA566" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB566" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC566" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD566" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE566" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="AF566" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG566" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AH566" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI566" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="AJ566" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK566" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL566" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM566" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="567" hidden="true">
+      <c r="A567" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="B567" s="2"/>
+      <c r="C567" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="D567" s="2"/>
+      <c r="E567" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F567" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="G567" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H567" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I567" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="J567" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K567" t="s" s="2">
+        <v>321</v>
+      </c>
+      <c r="L567" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="M567" s="2"/>
+      <c r="N567" s="2"/>
+      <c r="O567" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P567" s="2"/>
+      <c r="Q567" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R567" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S567" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T567" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U567" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V567" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W567" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X567" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y567" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z567" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA567" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB567" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC567" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD567" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE567" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="AF567" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG567" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AH567" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI567" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="AJ567" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK567" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL567" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM567" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="568" hidden="true">
+      <c r="A568" t="s" s="2">
+        <v>323</v>
+      </c>
+      <c r="B568" s="2"/>
+      <c r="C568" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="D568" s="2"/>
+      <c r="E568" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F568" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="G568" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H568" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I568" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="J568" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="K568" t="s" s="2">
+        <v>324</v>
+      </c>
+      <c r="L568" t="s" s="2">
+        <v>325</v>
+      </c>
+      <c r="M568" s="2"/>
+      <c r="N568" s="2"/>
+      <c r="O568" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P568" s="2"/>
+      <c r="Q568" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R568" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S568" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T568" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U568" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V568" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W568" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X568" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y568" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z568" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA568" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB568" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC568" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD568" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE568" t="s" s="2">
+        <v>323</v>
+      </c>
+      <c r="AF568" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG568" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AH568" t="s" s="2">
+        <v>326</v>
+      </c>
+      <c r="AI568" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="AJ568" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK568" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL568" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM568" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="569" hidden="true">
+      <c r="A569" t="s" s="2">
+        <v>327</v>
+      </c>
+      <c r="B569" s="2"/>
+      <c r="C569" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="D569" s="2"/>
+      <c r="E569" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F569" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="G569" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H569" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I569" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J569" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K569" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="L569" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="M569" s="2"/>
+      <c r="N569" s="2"/>
+      <c r="O569" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P569" s="2"/>
+      <c r="Q569" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R569" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S569" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T569" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U569" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V569" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W569" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X569" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y569" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z569" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA569" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB569" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC569" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD569" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE569" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AF569" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG569" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AH569" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI569" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AJ569" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK569" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="AL569" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM569" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="570" hidden="true">
+      <c r="A570" t="s" s="2">
+        <v>328</v>
+      </c>
+      <c r="B570" s="2"/>
+      <c r="C570" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="D570" s="2"/>
+      <c r="E570" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F570" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G570" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H570" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I570" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J570" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="K570" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="L570" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="M570" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="N570" s="2"/>
+      <c r="O570" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P570" s="2"/>
+      <c r="Q570" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R570" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S570" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T570" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U570" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V570" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W570" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X570" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y570" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z570" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA570" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB570" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC570" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD570" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE570" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="AF570" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG570" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH570" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI570" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="AJ570" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK570" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="AL570" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM570" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="571" hidden="true">
+      <c r="A571" t="s" s="2">
+        <v>329</v>
+      </c>
+      <c r="B571" s="2"/>
+      <c r="C571" t="s" s="2">
+        <v>246</v>
+      </c>
+      <c r="D571" s="2"/>
+      <c r="E571" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F571" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G571" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H571" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="I571" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="J571" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="K571" t="s" s="2">
+        <v>247</v>
+      </c>
+      <c r="L571" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="M571" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="N571" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="O571" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P571" s="2"/>
+      <c r="Q571" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R571" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S571" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T571" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U571" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V571" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W571" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X571" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y571" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z571" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA571" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB571" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC571" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD571" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE571" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="AF571" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG571" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH571" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI571" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="AJ571" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK571" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL571" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM571" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="572" hidden="true">
+      <c r="A572" t="s" s="2">
+        <v>330</v>
+      </c>
+      <c r="B572" s="2"/>
+      <c r="C572" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="D572" s="2"/>
+      <c r="E572" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="F572" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="G572" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H572" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I572" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="J572" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K572" t="s" s="2">
+        <v>331</v>
+      </c>
+      <c r="L572" t="s" s="2">
+        <v>332</v>
+      </c>
+      <c r="M572" s="2"/>
+      <c r="N572" s="2"/>
+      <c r="O572" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P572" s="2"/>
+      <c r="Q572" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R572" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S572" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T572" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U572" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V572" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W572" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X572" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y572" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z572" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA572" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB572" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC572" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD572" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE572" t="s" s="2">
+        <v>330</v>
+      </c>
+      <c r="AF572" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AG572" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AH572" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI572" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="AJ572" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK572" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL572" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM572" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="573" hidden="true">
+      <c r="A573" t="s" s="2">
+        <v>333</v>
+      </c>
+      <c r="B573" s="2"/>
+      <c r="C573" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="D573" s="2"/>
+      <c r="E573" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F573" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="G573" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H573" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I573" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="J573" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="K573" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="L573" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="M573" s="2"/>
+      <c r="N573" s="2"/>
+      <c r="O573" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P573" s="2"/>
+      <c r="Q573" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R573" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S573" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T573" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U573" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V573" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W573" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X573" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y573" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z573" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA573" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB573" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC573" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD573" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE573" t="s" s="2">
+        <v>333</v>
+      </c>
+      <c r="AF573" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG573" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AH573" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI573" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="AJ573" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK573" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL573" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM573" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="574" hidden="true">
+      <c r="A574" t="s" s="2">
+        <v>336</v>
+      </c>
+      <c r="B574" s="2"/>
+      <c r="C574" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="D574" s="2"/>
+      <c r="E574" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F574" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="G574" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H574" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I574" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="J574" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K574" t="s" s="2">
+        <v>337</v>
+      </c>
+      <c r="L574" t="s" s="2">
+        <v>338</v>
+      </c>
+      <c r="M574" t="s" s="2">
+        <v>339</v>
+      </c>
+      <c r="N574" s="2"/>
+      <c r="O574" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P574" s="2"/>
+      <c r="Q574" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R574" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S574" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T574" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U574" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V574" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W574" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X574" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y574" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z574" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA574" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB574" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC574" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD574" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE574" t="s" s="2">
+        <v>336</v>
+      </c>
+      <c r="AF574" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG574" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AH574" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI574" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="AJ574" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK574" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL574" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM574" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="575" hidden="true">
+      <c r="A575" t="s" s="2">
+        <v>340</v>
+      </c>
+      <c r="B575" s="2"/>
+      <c r="C575" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="D575" s="2"/>
+      <c r="E575" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F575" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="G575" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H575" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I575" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="J575" t="s" s="2">
+        <v>119</v>
+      </c>
+      <c r="K575" t="s" s="2">
+        <v>341</v>
+      </c>
+      <c r="L575" t="s" s="2">
+        <v>342</v>
+      </c>
+      <c r="M575" t="s" s="2">
+        <v>343</v>
+      </c>
+      <c r="N575" s="2"/>
+      <c r="O575" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P575" s="2"/>
+      <c r="Q575" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R575" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S575" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T575" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U575" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V575" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W575" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X575" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y575" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z575" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA575" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB575" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC575" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD575" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE575" t="s" s="2">
+        <v>340</v>
+      </c>
+      <c r="AF575" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG575" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AH575" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI575" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="AJ575" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK575" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL575" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM575" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="576" hidden="true">
+      <c r="A576" t="s" s="2">
+        <v>344</v>
+      </c>
+      <c r="B576" s="2"/>
+      <c r="C576" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="D576" s="2"/>
+      <c r="E576" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F576" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="G576" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H576" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I576" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="J576" t="s" s="2">
+        <v>275</v>
+      </c>
+      <c r="K576" t="s" s="2">
+        <v>345</v>
+      </c>
+      <c r="L576" t="s" s="2">
+        <v>346</v>
+      </c>
+      <c r="M576" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="N576" s="2"/>
+      <c r="O576" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P576" s="2"/>
+      <c r="Q576" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R576" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S576" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T576" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U576" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V576" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W576" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X576" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y576" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z576" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA576" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB576" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC576" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD576" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE576" t="s" s="2">
+        <v>344</v>
+      </c>
+      <c r="AF576" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG576" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AH576" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI576" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AJ576" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK576" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL576" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM576" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="577" hidden="true">
+      <c r="A577" t="s" s="2">
+        <v>447</v>
+      </c>
+      <c r="B577" s="2"/>
+      <c r="C577" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="D577" s="2"/>
+      <c r="E577" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F577" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="G577" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H577" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I577" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="J577" t="s" s="2">
+        <v>448</v>
+      </c>
+      <c r="K577" t="s" s="2">
+        <v>449</v>
+      </c>
+      <c r="L577" t="s" s="2">
+        <v>450</v>
+      </c>
+      <c r="M577" t="s" s="2">
+        <v>451</v>
+      </c>
+      <c r="N577" t="s" s="2">
+        <v>452</v>
+      </c>
+      <c r="O577" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="P577" s="2"/>
+      <c r="Q577" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="R577" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S577" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T577" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U577" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V577" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W577" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X577" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y577" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z577" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA577" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB577" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC577" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD577" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE577" t="s" s="2">
+        <v>447</v>
+      </c>
+      <c r="AF577" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG577" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AH577" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI577" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="AJ577" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK577" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL577" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM577" t="s" s="2">
         <v>74</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AM545">
+  <autoFilter ref="A1:AM577">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -61929,7 +65479,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI544">
+  <conditionalFormatting sqref="A2:AI576">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>